<commit_message>
Incorporate design review feedback - Enhance routing of input path - Remove voltage reference, used voltage divider instead for gain voltage - Made vias smaller
</commit_message>
<xml_diff>
--- a/docs/bom.xlsx
+++ b/docs/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
   <si>
     <t xml:space="preserve">Bill of Materials (BOM)</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Project: current_probe</t>
   </si>
   <si>
-    <t xml:space="preserve">Version: 07.10.2023</t>
+    <t xml:space="preserve">Version: 08.10.2023</t>
   </si>
   <si>
     <t xml:space="preserve">Item</t>
@@ -46,9 +46,15 @@
     <t xml:space="preserve">Footprint</t>
   </si>
   <si>
+    <t xml:space="preserve">Part. No.</t>
+  </si>
+  <si>
     <t xml:space="preserve">DNP</t>
   </si>
   <si>
+    <t xml:space="preserve">Datasheet</t>
+  </si>
+  <si>
     <t xml:space="preserve">C1</t>
   </si>
   <si>
@@ -58,6 +64,9 @@
     <t xml:space="preserve">Capacitor_SMD:C_0603_1608Metric</t>
   </si>
   <si>
+    <t xml:space="preserve">~</t>
+  </si>
+  <si>
     <t xml:space="preserve">C2</t>
   </si>
   <si>
@@ -82,7 +91,7 @@
     <t xml:space="preserve">1n</t>
   </si>
   <si>
-    <t xml:space="preserve">C21, C27, C28, C33</t>
+    <t xml:space="preserve">C21, C27, C28, C32</t>
   </si>
   <si>
     <t xml:space="preserve">10u</t>
@@ -91,7 +100,7 @@
     <t xml:space="preserve">Capacitor_SMD:C_0805_2012Metric</t>
   </si>
   <si>
-    <t xml:space="preserve">C22, C31, C32</t>
+    <t xml:space="preserve">C22, C31, C33</t>
   </si>
   <si>
     <t xml:space="preserve">1u</t>
@@ -124,6 +133,9 @@
     <t xml:space="preserve">Diode_SMD:D_0603_1608Metric</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.onsemi.com/pub/Collateral/ESD9B-D.PDF</t>
+  </si>
+  <si>
     <t xml:space="preserve">D2</t>
   </si>
   <si>
@@ -136,7 +148,7 @@
     <t xml:space="preserve">D3</t>
   </si>
   <si>
-    <t xml:space="preserve">LED</t>
+    <t xml:space="preserve">GREEN</t>
   </si>
   <si>
     <t xml:space="preserve">LED_SMD:LED_0805_2012Metric</t>
@@ -145,21 +157,36 @@
     <t xml:space="preserve">F1</t>
   </si>
   <si>
-    <t xml:space="preserve">250mA</t>
+    <t xml:space="preserve">300 mA</t>
   </si>
   <si>
     <t xml:space="preserve">Fuse:Fuse_0805_2012Metric</t>
   </si>
   <si>
-    <t xml:space="preserve">FB1, FB2, FB3, FB4, FB5, FB6, FB7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLM21</t>
+    <t xml:space="preserve">0805L010/24YR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB1, FB2, FB3</t>
   </si>
   <si>
     <t xml:space="preserve">Inductor_SMD:L_0603_1608Metric</t>
   </si>
   <si>
+    <t xml:space="preserve">BLM18SD220SN1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.murata.com/en-us/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB4, FB5, FB6, FB7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2k2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLM18BD222SZ1D</t>
+  </si>
+  <si>
     <t xml:space="preserve">J1</t>
   </si>
   <si>
@@ -169,6 +196,12 @@
     <t xml:space="preserve">Connector_Coaxial:SMA_Amphenol_132289_EdgeMount</t>
   </si>
   <si>
+    <t xml:space="preserve">132289RP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://s3-us-west-2.amazonaws.com/catsy.582/132289rp.pdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">J2</t>
   </si>
   <si>
@@ -205,12 +238,18 @@
     <t xml:space="preserve">Inductor_SMD:L_0805_2012Metric</t>
   </si>
   <si>
+    <t xml:space="preserve">MLZ2012N101LT000</t>
+  </si>
+  <si>
     <t xml:space="preserve">L3</t>
   </si>
   <si>
     <t xml:space="preserve">6u8</t>
   </si>
   <si>
+    <t xml:space="preserve">MLZ2012N6R8LT000</t>
+  </si>
+  <si>
     <t xml:space="preserve">PS1</t>
   </si>
   <si>
@@ -220,60 +259,66 @@
     <t xml:space="preserve">Converter_DCDC:Converter_DCDC_Murata_MEE1SxxxxSC_THT</t>
   </si>
   <si>
-    <t xml:space="preserve">R1, R2, R6, R7</t>
+    <t xml:space="preserve">https://power.murata.com/pub/data/power/ncl/kdc_mee1.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor_SMD:R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R3, R8, R9</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistor_SMD:R_0603_1608Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4, R5, R11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4k7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9</t>
+    <t xml:space="preserve">R4, R7, R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5, R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3k</t>
   </si>
   <si>
     <t xml:space="preserve">Potentiometer_THT:Potentiometer_Bourns_3296Y_Vertical</t>
   </si>
   <si>
-    <t xml:space="preserve">R10</t>
+    <t xml:space="preserve">3296Y-1-302LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bourns.com/docs/product-datasheets/3296.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12</t>
   </si>
   <si>
     <t xml:space="preserve">RCLMP</t>
   </si>
   <si>
-    <t xml:space="preserve">R12, R13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP1, TP4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keystone 5001</t>
+    <t xml:space="preserve">TP1, TP2, TP3, TP4, TP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestPoint</t>
   </si>
   <si>
     <t xml:space="preserve">TestPoint:TestPoint_Loop_D1.80mm_Drill1.0mm_Beaded</t>
   </si>
   <si>
-    <t xml:space="preserve">TP2, TP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestPoint:TestPoint_Keystone_5000-5004_Miniature</t>
-  </si>
-  <si>
     <t xml:space="preserve">TR1</t>
   </si>
   <si>
@@ -283,6 +328,9 @@
     <t xml:space="preserve">RF_Mini-Circuits:Mini-Circuits_CD637_H5.23mm</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.minicircuits.com/pdfs/ADTT1-6+.pdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">U1</t>
   </si>
   <si>
@@ -293,15 +341,6 @@
   </si>
   <si>
     <t xml:space="preserve">U2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADR510ARTZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3</t>
   </si>
   <si>
     <t xml:space="preserve">ADM7150ARDZ-5.0</t>
@@ -322,6 +361,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -343,18 +383,21 @@
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -411,8 +454,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,32 +471,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -525,155 +572,199 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J19" activeCellId="0" sqref="J19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="43.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="58.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="72.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="I7" s="0"/>
+    </row>
+    <row r="8" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
+      <c r="D8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+    </row>
+    <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
+      <c r="F9" s="0"/>
+      <c r="G9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+    </row>
+    <row r="10" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -683,13 +774,16 @@
         <v>11</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,13 +794,16 @@
         <v>8</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,13 +814,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,13 +834,16 @@
         <v>3</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,13 +854,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,13 +874,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,13 +894,16 @@
         <v>1</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,13 +914,16 @@
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,13 +934,16 @@
         <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,13 +954,16 @@
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,13 +974,19 @@
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,37 +994,51 @@
         <v>15</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+      <c r="D22" s="8" t="n">
+        <v>22</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B23" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="B23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="0"/>
+      <c r="H23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="0"/>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -907,13 +1048,19 @@
         <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,13 +1071,16 @@
         <v>1</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -938,16 +1088,19 @@
         <v>19</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,13 +1111,16 @@
         <v>2</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>60</v>
+        <v>68</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,16 +1128,22 @@
         <v>21</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>60</v>
+        <v>71</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,70 +1154,98 @@
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="n">
+        <v>71</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B30" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="n">
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+    </row>
+    <row r="31" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B31" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="B31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>25</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="8" t="n">
-        <v>330</v>
+        <v>83</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,16 +1253,19 @@
         <v>26</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>73</v>
+        <v>85</v>
+      </c>
+      <c r="D33" s="8" t="n">
+        <v>330</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>68</v>
+        <v>82</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,53 +1273,68 @@
         <v>27</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>73</v>
+        <v>86</v>
+      </c>
+      <c r="D34" s="8" t="n">
+        <v>237</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="n">
+        <v>82</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B35" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>29</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="8" t="n">
-        <v>237</v>
+        <v>89</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>68</v>
+        <v>91</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,16 +1342,22 @@
         <v>30</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,16 +1365,22 @@
         <v>31</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>83</v>
+        <v>98</v>
+      </c>
+      <c r="F38" s="8" t="n">
+        <v>5001</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,13 +1391,19 @@
         <v>1</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>86</v>
+        <v>101</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,14 +1414,18 @@
         <v>1</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>89</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -1205,31 +1435,26 @@
         <v>1</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>92</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="B42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>95</v>
-      </c>
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="H42" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>